<commit_message>
data clean, imputation, for analysis jupyter notebook
Happiness Index, GDP, Social Support, Life Expectancy, Freedom, Generosity, Trust(Perception of Corruption),  + Vivi's data sets used for sampling & imputation (filled NaN values)
</commit_message>
<xml_diff>
--- a/Project Summary.xlsx
+++ b/Project Summary.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytakeda-my.sharepoint.com/personal/sheri_shojaie_takeda_com/Documents/Documents/__DS Bootcamp/Project/Sheri Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECFDAA2B-85CC-470C-8E14-910ABCE60162}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{ECFDAA2B-85CC-470C-8E14-910ABCE60162}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{93E3D492-A18A-41FE-A407-9F95ED3A78BF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{D081F38E-7123-48AD-BD94-A1191E194800}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Countries" sheetId="2" r:id="rId2"/>
-    <sheet name="Data frame" sheetId="3" r:id="rId3"/>
+    <sheet name="Dataframe_main" sheetId="3" r:id="rId3"/>
+    <sheet name="Dataframe_matrix format" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$B$3:$E$3</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="81">
   <si>
     <t>Independent variable</t>
   </si>
@@ -149,13 +150,7 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>year 1</t>
-  </si>
-  <si>
-    <t>year 2</t>
+    <t>year</t>
   </si>
   <si>
     <t>Needs to be pulled</t>
@@ -165,6 +160,126 @@
   </si>
   <si>
     <t>Variable type</t>
+  </si>
+  <si>
+    <t>ISO code</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Country name</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Country name 1</t>
+  </si>
+  <si>
+    <t>Country name 2</t>
+  </si>
+  <si>
+    <t>BCD</t>
+  </si>
+  <si>
+    <t>Country 1</t>
+  </si>
+  <si>
+    <t>Country 2</t>
+  </si>
+  <si>
+    <t>Year 1</t>
+  </si>
+  <si>
+    <t>Year 2</t>
+  </si>
+  <si>
+    <t>Sum of Life Ladder</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
@@ -188,7 +303,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -211,26 +326,193 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="65"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -540,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEA49E3-C43C-47D7-AED7-F4048A0B4EFE}">
-  <dimension ref="B3:G29"/>
+  <dimension ref="B3:H29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,18 +833,18 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" customWidth="1"/>
     <col min="7" max="7" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>3</v>
@@ -570,10 +852,11 @@
       <c r="E3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -583,175 +866,177 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>2019</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>2019</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -762,10 +1047,10 @@
       <c r="C17" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -776,10 +1061,10 @@
       <c r="C18" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -790,10 +1075,10 @@
       <c r="C19" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -804,10 +1089,10 @@
       <c r="C20" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -818,11 +1103,11 @@
       <c r="C21" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>40</v>
+      <c r="E21" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -832,11 +1117,11 @@
       <c r="C22" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>40</v>
+      <c r="E22" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -846,11 +1131,11 @@
       <c r="C23" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>40</v>
+      <c r="E23" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -860,11 +1145,11 @@
       <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>40</v>
+      <c r="E24" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -874,11 +1159,11 @@
       <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>40</v>
+      <c r="E25" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -888,11 +1173,11 @@
       <c r="C26" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>40</v>
+      <c r="E26" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -902,11 +1187,11 @@
       <c r="C27" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>40</v>
+      <c r="E27" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -916,7 +1201,7 @@
       <c r="C28" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -927,10 +1212,10 @@
       <c r="C29" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="2">
         <v>2018</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -942,24 +1227,2566 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD03779B-1072-4284-A0C9-AE27034BE457}">
-  <dimension ref="A1"/>
+  <dimension ref="B4:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="9"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2005</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2006</v>
+      </c>
+      <c r="E5" s="10">
+        <v>2007</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2008</v>
+      </c>
+      <c r="G5" s="10">
+        <v>2009</v>
+      </c>
+      <c r="H5" s="10">
+        <v>2010</v>
+      </c>
+      <c r="I5" s="10">
+        <v>2011</v>
+      </c>
+      <c r="J5" s="10">
+        <v>2012</v>
+      </c>
+      <c r="K5" s="10">
+        <v>2013</v>
+      </c>
+      <c r="L5" s="10">
+        <v>2014</v>
+      </c>
+      <c r="M5" s="10">
+        <v>2015</v>
+      </c>
+      <c r="N5" s="10">
+        <v>2016</v>
+      </c>
+      <c r="O5" s="10">
+        <v>2017</v>
+      </c>
+      <c r="P5" s="10">
+        <v>2018</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>2019</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13">
+        <v>6.3129253387451172</v>
+      </c>
+      <c r="E6" s="13">
+        <v>6.0731582641601563</v>
+      </c>
+      <c r="F6" s="13">
+        <v>5.9610342979431152</v>
+      </c>
+      <c r="G6" s="13">
+        <v>6.42413330078125</v>
+      </c>
+      <c r="H6" s="13">
+        <v>6.4410672187805176</v>
+      </c>
+      <c r="I6" s="13">
+        <v>6.7758054733276367</v>
+      </c>
+      <c r="J6" s="13">
+        <v>6.4683871269226074</v>
+      </c>
+      <c r="K6" s="13">
+        <v>6.5822601318359375</v>
+      </c>
+      <c r="L6" s="13">
+        <v>6.671114444732666</v>
+      </c>
+      <c r="M6" s="13">
+        <v>6.6971306800842285</v>
+      </c>
+      <c r="N6" s="13">
+        <v>6.4272212982177734</v>
+      </c>
+      <c r="O6" s="13">
+        <v>6.039330005645752</v>
+      </c>
+      <c r="P6" s="13">
+        <v>5.7927966117858887</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>6.0855607986450195</v>
+      </c>
+      <c r="R6" s="14">
+        <v>88.751924991607666</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="16">
+        <v>7.3406882286071777</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17">
+        <v>7.2853908538818359</v>
+      </c>
+      <c r="F7" s="17">
+        <v>7.2537574768066406</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17">
+        <v>7.4500470161437988</v>
+      </c>
+      <c r="I7" s="17">
+        <v>7.405616283416748</v>
+      </c>
+      <c r="J7" s="17">
+        <v>7.1955857276916504</v>
+      </c>
+      <c r="K7" s="17">
+        <v>7.3641691207885742</v>
+      </c>
+      <c r="L7" s="17">
+        <v>7.2885503768920898</v>
+      </c>
+      <c r="M7" s="17">
+        <v>7.3090605735778809</v>
+      </c>
+      <c r="N7" s="17">
+        <v>7.2500801086425781</v>
+      </c>
+      <c r="O7" s="17">
+        <v>7.2570376396179199</v>
+      </c>
+      <c r="P7" s="17">
+        <v>7.1769933700561523</v>
+      </c>
+      <c r="Q7" s="17">
+        <v>7.2339949607849121</v>
+      </c>
+      <c r="R7" s="18">
+        <v>94.810971736907959</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17">
+        <v>4.3189091682434082</v>
+      </c>
+      <c r="E8" s="17">
+        <v>4.6073222160339355</v>
+      </c>
+      <c r="F8" s="17">
+        <v>5.0522785186767578</v>
+      </c>
+      <c r="G8" s="17">
+        <v>5.0828514099121094</v>
+      </c>
+      <c r="H8" s="17">
+        <v>4.8584814071655273</v>
+      </c>
+      <c r="I8" s="17">
+        <v>4.9856491088867188</v>
+      </c>
+      <c r="J8" s="17">
+        <v>4.7244439125061035</v>
+      </c>
+      <c r="K8" s="17">
+        <v>4.660161018371582</v>
+      </c>
+      <c r="L8" s="17">
+        <v>4.6355648040771484</v>
+      </c>
+      <c r="M8" s="17">
+        <v>4.6334738731384277</v>
+      </c>
+      <c r="N8" s="17">
+        <v>4.5561408996582031</v>
+      </c>
+      <c r="O8" s="17">
+        <v>4.3097710609436035</v>
+      </c>
+      <c r="P8" s="17">
+        <v>4.4992170333862305</v>
+      </c>
+      <c r="Q8" s="17">
+        <v>5.1142168045043945</v>
+      </c>
+      <c r="R8" s="18">
+        <v>66.03848123550415</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="16">
+        <v>6.6367712020874023</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17">
+        <v>6.3206729888916016</v>
+      </c>
+      <c r="F9" s="17">
+        <v>6.6914248466491699</v>
+      </c>
+      <c r="G9" s="17">
+        <v>7.0008316040039063</v>
+      </c>
+      <c r="H9" s="17">
+        <v>6.8373312950134277</v>
+      </c>
+      <c r="I9" s="17">
+        <v>7.0378165245056152</v>
+      </c>
+      <c r="J9" s="17">
+        <v>6.660003662109375</v>
+      </c>
+      <c r="K9" s="17">
+        <v>7.1402826309204102</v>
+      </c>
+      <c r="L9" s="17">
+        <v>6.9809989929199219</v>
+      </c>
+      <c r="M9" s="17">
+        <v>6.5468969345092773</v>
+      </c>
+      <c r="N9" s="17">
+        <v>6.3748173713684082</v>
+      </c>
+      <c r="O9" s="17">
+        <v>6.3329291343688965</v>
+      </c>
+      <c r="P9" s="17">
+        <v>6.1909217834472656</v>
+      </c>
+      <c r="Q9" s="17">
+        <v>6.4511489868164063</v>
+      </c>
+      <c r="R9" s="18">
+        <v>93.202847957611084</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="16">
+        <v>7.4180483818054199</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17">
+        <v>7.481752872467041</v>
+      </c>
+      <c r="F10" s="17">
+        <v>7.4856038093566895</v>
+      </c>
+      <c r="G10" s="17">
+        <v>7.4878244400024414</v>
+      </c>
+      <c r="H10" s="17">
+        <v>7.6503462791442871</v>
+      </c>
+      <c r="I10" s="17">
+        <v>7.426053524017334</v>
+      </c>
+      <c r="J10" s="17">
+        <v>7.4151444435119629</v>
+      </c>
+      <c r="K10" s="17">
+        <v>7.5937938690185547</v>
+      </c>
+      <c r="L10" s="17">
+        <v>7.304257869720459</v>
+      </c>
+      <c r="M10" s="17">
+        <v>7.4127726554870605</v>
+      </c>
+      <c r="N10" s="17">
+        <v>7.2448458671569824</v>
+      </c>
+      <c r="O10" s="17">
+        <v>7.4148683547973633</v>
+      </c>
+      <c r="P10" s="17">
+        <v>7.1754965782165527</v>
+      </c>
+      <c r="Q10" s="17">
+        <v>7.1090764999389648</v>
+      </c>
+      <c r="R10" s="18">
+        <v>103.61988544464111</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17">
+        <v>4.5604953765869141</v>
+      </c>
+      <c r="E11" s="17">
+        <v>4.8628621101379395</v>
+      </c>
+      <c r="F11" s="17">
+        <v>4.8462948799133301</v>
+      </c>
+      <c r="G11" s="17">
+        <v>4.4543609619140625</v>
+      </c>
+      <c r="H11" s="17">
+        <v>4.6527366638183594</v>
+      </c>
+      <c r="I11" s="17">
+        <v>5.0372076034545898</v>
+      </c>
+      <c r="J11" s="17">
+        <v>5.0949172973632813</v>
+      </c>
+      <c r="K11" s="17">
+        <v>5.2410902976989746</v>
+      </c>
+      <c r="L11" s="17">
+        <v>5.1956191062927246</v>
+      </c>
+      <c r="M11" s="17">
+        <v>5.3038778305053711</v>
+      </c>
+      <c r="N11" s="17">
+        <v>5.324955940246582</v>
+      </c>
+      <c r="O11" s="17">
+        <v>5.0990614891052246</v>
+      </c>
+      <c r="P11" s="17">
+        <v>5.1314339637756348</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>5.1441202163696289</v>
+      </c>
+      <c r="R11" s="18">
+        <v>69.949033737182617</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="16">
+        <v>8.0189342498779297</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17">
+        <v>7.834233283996582</v>
+      </c>
+      <c r="F12" s="17">
+        <v>7.9708919525146484</v>
+      </c>
+      <c r="G12" s="17">
+        <v>7.6833586692810059</v>
+      </c>
+      <c r="H12" s="17">
+        <v>7.7705154418945313</v>
+      </c>
+      <c r="I12" s="17">
+        <v>7.7882318496704102</v>
+      </c>
+      <c r="J12" s="17">
+        <v>7.5199093818664551</v>
+      </c>
+      <c r="K12" s="17">
+        <v>7.5886068344116211</v>
+      </c>
+      <c r="L12" s="17">
+        <v>7.5075592994689941</v>
+      </c>
+      <c r="M12" s="17">
+        <v>7.5144248008728027</v>
+      </c>
+      <c r="N12" s="17">
+        <v>7.5577826499938965</v>
+      </c>
+      <c r="O12" s="17">
+        <v>7.5937023162841797</v>
+      </c>
+      <c r="P12" s="17">
+        <v>7.6487855911254883</v>
+      </c>
+      <c r="Q12" s="17">
+        <v>7.6930031776428223</v>
+      </c>
+      <c r="R12" s="18">
+        <v>107.68993949890137</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17">
+        <v>7.6724491119384766</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17">
+        <v>7.6706266403198242</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17">
+        <v>7.3932642936706543</v>
+      </c>
+      <c r="I13" s="17">
+        <v>7.3542251586914063</v>
+      </c>
+      <c r="J13" s="17">
+        <v>7.4202094078063965</v>
+      </c>
+      <c r="K13" s="17">
+        <v>7.4446358680725098</v>
+      </c>
+      <c r="L13" s="17">
+        <v>7.3845710754394531</v>
+      </c>
+      <c r="M13" s="17">
+        <v>7.4479255676269531</v>
+      </c>
+      <c r="N13" s="17">
+        <v>7.6598434448242188</v>
+      </c>
+      <c r="O13" s="17">
+        <v>7.7882518768310547</v>
+      </c>
+      <c r="P13" s="17">
+        <v>7.8581070899963379</v>
+      </c>
+      <c r="Q13" s="17">
+        <v>7.7803478240966797</v>
+      </c>
+      <c r="R13" s="18">
+        <v>90.874457359313965</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="16">
+        <v>7.0933928489685059</v>
+      </c>
+      <c r="D14" s="17">
+        <v>6.582700252532959</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17">
+        <v>7.0080647468566895</v>
+      </c>
+      <c r="G14" s="17">
+        <v>6.2834982872009277</v>
+      </c>
+      <c r="H14" s="17">
+        <v>6.7979011535644531</v>
+      </c>
+      <c r="I14" s="17">
+        <v>6.9591851234436035</v>
+      </c>
+      <c r="J14" s="17">
+        <v>6.6493654251098633</v>
+      </c>
+      <c r="K14" s="17">
+        <v>6.667121410369873</v>
+      </c>
+      <c r="L14" s="17">
+        <v>6.4668679237365723</v>
+      </c>
+      <c r="M14" s="17">
+        <v>6.3576250076293945</v>
+      </c>
+      <c r="N14" s="17">
+        <v>6.4752087593078613</v>
+      </c>
+      <c r="O14" s="17">
+        <v>6.6352224349975586</v>
+      </c>
+      <c r="P14" s="17">
+        <v>6.6659035682678223</v>
+      </c>
+      <c r="Q14" s="17">
+        <v>6.6896443367004395</v>
+      </c>
+      <c r="R14" s="18">
+        <v>93.331701278686523</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="16">
+        <v>6.6195497512817383</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17">
+        <v>6.4168195724487305</v>
+      </c>
+      <c r="F15" s="17">
+        <v>6.5217900276184082</v>
+      </c>
+      <c r="G15" s="17">
+        <v>6.6414933204650879</v>
+      </c>
+      <c r="H15" s="17">
+        <v>6.7245311737060547</v>
+      </c>
+      <c r="I15" s="17">
+        <v>6.621312141418457</v>
+      </c>
+      <c r="J15" s="17">
+        <v>6.702362060546875</v>
+      </c>
+      <c r="K15" s="17">
+        <v>6.9651250839233398</v>
+      </c>
+      <c r="L15" s="17">
+        <v>6.9842143058776855</v>
+      </c>
+      <c r="M15" s="17">
+        <v>7.037137508392334</v>
+      </c>
+      <c r="N15" s="17">
+        <v>6.8737630844116211</v>
+      </c>
+      <c r="O15" s="17">
+        <v>7.0743246078491211</v>
+      </c>
+      <c r="P15" s="17">
+        <v>7.1183643341064453</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>7.0354723930358887</v>
+      </c>
+      <c r="R15" s="18">
+        <v>95.336259365081787</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17">
+        <v>5.3482589721679688</v>
+      </c>
+      <c r="E16" s="17">
+        <v>5.0267934799194336</v>
+      </c>
+      <c r="F16" s="17">
+        <v>5.1458330154418945</v>
+      </c>
+      <c r="G16" s="17">
+        <v>4.5215177536010742</v>
+      </c>
+      <c r="H16" s="17">
+        <v>4.9892773628234863</v>
+      </c>
+      <c r="I16" s="17">
+        <v>4.6348714828491211</v>
+      </c>
+      <c r="J16" s="17">
+        <v>4.720146656036377</v>
+      </c>
+      <c r="K16" s="17">
+        <v>4.4277887344360352</v>
+      </c>
+      <c r="L16" s="17">
+        <v>4.4243793487548828</v>
+      </c>
+      <c r="M16" s="17">
+        <v>4.3420791625976563</v>
+      </c>
+      <c r="N16" s="17">
+        <v>4.1791772842407227</v>
+      </c>
+      <c r="O16" s="17">
+        <v>4.0461111068725586</v>
+      </c>
+      <c r="P16" s="17">
+        <v>3.8180687427520752</v>
+      </c>
+      <c r="Q16" s="17">
+        <v>3.2487697601318359</v>
+      </c>
+      <c r="R16" s="18">
+        <v>62.873072862625122</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17">
+        <v>4.9469780921936035</v>
+      </c>
+      <c r="E17" s="17">
+        <v>5.1012139320373535</v>
+      </c>
+      <c r="F17" s="17">
+        <v>4.8153095245361328</v>
+      </c>
+      <c r="G17" s="17">
+        <v>5.4723610877990723</v>
+      </c>
+      <c r="H17" s="17">
+        <v>5.4572992324829102</v>
+      </c>
+      <c r="I17" s="17">
+        <v>5.1726083755493164</v>
+      </c>
+      <c r="J17" s="17">
+        <v>5.3677740097045898</v>
+      </c>
+      <c r="K17" s="17">
+        <v>5.2922377586364746</v>
+      </c>
+      <c r="L17" s="17">
+        <v>5.5973753929138184</v>
+      </c>
+      <c r="M17" s="17">
+        <v>5.0427999496459961</v>
+      </c>
+      <c r="N17" s="17">
+        <v>5.1363253593444824</v>
+      </c>
+      <c r="O17" s="17">
+        <v>5.0984015464782715</v>
+      </c>
+      <c r="P17" s="17">
+        <v>5.3402957916259766</v>
+      </c>
+      <c r="Q17" s="17">
+        <v>5.3465127944946289</v>
+      </c>
+      <c r="R17" s="18">
+        <v>73.187492847442627</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="16">
+        <v>5.3081903457641602</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17">
+        <v>5.3363714218139648</v>
+      </c>
+      <c r="F18" s="17">
+        <v>5.1289882659912109</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17">
+        <v>4.7675070762634277</v>
+      </c>
+      <c r="J18" s="17">
+        <v>4.6089277267456055</v>
+      </c>
+      <c r="K18" s="17">
+        <v>5.1395792961120605</v>
+      </c>
+      <c r="L18" s="17">
+        <v>4.6822242736816406</v>
+      </c>
+      <c r="M18" s="17">
+        <v>4.7499556541442871</v>
+      </c>
+      <c r="N18" s="17">
+        <v>4.6527309417724609</v>
+      </c>
+      <c r="O18" s="17">
+        <v>4.7167830467224121</v>
+      </c>
+      <c r="P18" s="17">
+        <v>4.2781176567077637</v>
+      </c>
+      <c r="Q18" s="17">
+        <v>5.0061459541320801</v>
+      </c>
+      <c r="R18" s="18">
+        <v>58.375521659851074</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="16">
+        <v>6.8537836074829102</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17">
+        <v>6.5744123458862305</v>
+      </c>
+      <c r="F19" s="17">
+        <v>6.7797741889953613</v>
+      </c>
+      <c r="G19" s="17">
+        <v>6.3338003158569336</v>
+      </c>
+      <c r="H19" s="17">
+        <v>6.3542380332946777</v>
+      </c>
+      <c r="I19" s="17">
+        <v>6.0570864677429199</v>
+      </c>
+      <c r="J19" s="17">
+        <v>5.8393139839172363</v>
+      </c>
+      <c r="K19" s="17">
+        <v>6.009373664855957</v>
+      </c>
+      <c r="L19" s="17">
+        <v>6.0265851020812988</v>
+      </c>
+      <c r="M19" s="17">
+        <v>5.8476839065551758</v>
+      </c>
+      <c r="N19" s="17">
+        <v>5.954524040222168</v>
+      </c>
+      <c r="O19" s="17">
+        <v>6.1988701820373535</v>
+      </c>
+      <c r="P19" s="17">
+        <v>6.5165266990661621</v>
+      </c>
+      <c r="Q19" s="17">
+        <v>6.4454169273376465</v>
+      </c>
+      <c r="R19" s="18">
+        <v>87.791389465332031</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="16">
+        <v>6.5158171653747559</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17">
+        <v>6.2381978034973145</v>
+      </c>
+      <c r="F20" s="17">
+        <v>5.9106793403625488</v>
+      </c>
+      <c r="G20" s="17">
+        <v>5.8449993133544922</v>
+      </c>
+      <c r="H20" s="17">
+        <v>6.0567526817321777</v>
+      </c>
+      <c r="I20" s="17">
+        <v>6.2627935409545898</v>
+      </c>
+      <c r="J20" s="17">
+        <v>5.9682164192199707</v>
+      </c>
+      <c r="K20" s="17">
+        <v>5.9593615531921387</v>
+      </c>
+      <c r="L20" s="17">
+        <v>5.9226207733154297</v>
+      </c>
+      <c r="M20" s="17">
+        <v>5.8796844482421875</v>
+      </c>
+      <c r="N20" s="17">
+        <v>5.95465087890625</v>
+      </c>
+      <c r="O20" s="17">
+        <v>5.9106764793395996</v>
+      </c>
+      <c r="P20" s="17">
+        <v>5.7935752868652344</v>
+      </c>
+      <c r="Q20" s="17">
+        <v>5.9080390930175781</v>
+      </c>
+      <c r="R20" s="18">
+        <v>84.126064777374268</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17">
+        <v>6.0117168426513672</v>
+      </c>
+      <c r="E21" s="17">
+        <v>6.2389044761657715</v>
+      </c>
+      <c r="F21" s="17">
+        <v>5.8067817687988281</v>
+      </c>
+      <c r="G21" s="17">
+        <v>5.3847017288208008</v>
+      </c>
+      <c r="H21" s="17">
+        <v>5.5802817344665527</v>
+      </c>
+      <c r="I21" s="17">
+        <v>5.7863674163818359</v>
+      </c>
+      <c r="J21" s="17">
+        <v>5.9142837524414063</v>
+      </c>
+      <c r="K21" s="17">
+        <v>5.7701997756958008</v>
+      </c>
+      <c r="L21" s="17">
+        <v>5.9629216194152832</v>
+      </c>
+      <c r="M21" s="17">
+        <v>6.3221211433410645</v>
+      </c>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17">
+        <v>5.3388175964355469</v>
+      </c>
+      <c r="Q21" s="17">
+        <v>5.4279541969299316</v>
+      </c>
+      <c r="R21" s="18">
+        <v>69.545052051544189</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="16">
+        <v>6.580657958984375</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17">
+        <v>6.5253782272338867</v>
+      </c>
+      <c r="F22" s="17">
+        <v>6.8290362358093262</v>
+      </c>
+      <c r="G22" s="17">
+        <v>6.9628190994262695</v>
+      </c>
+      <c r="H22" s="17">
+        <v>6.8023886680603027</v>
+      </c>
+      <c r="I22" s="17">
+        <v>6.909515380859375</v>
+      </c>
+      <c r="J22" s="17">
+        <v>7.3201851844787598</v>
+      </c>
+      <c r="K22" s="17">
+        <v>7.4425463676452637</v>
+      </c>
+      <c r="L22" s="17">
+        <v>6.6798310279846191</v>
+      </c>
+      <c r="M22" s="17">
+        <v>6.2362871170043945</v>
+      </c>
+      <c r="N22" s="17">
+        <v>6.8241729736328125</v>
+      </c>
+      <c r="O22" s="17">
+        <v>6.4102993011474609</v>
+      </c>
+      <c r="P22" s="17">
+        <v>6.5495786666870117</v>
+      </c>
+      <c r="Q22" s="17">
+        <v>6.4319453239440918</v>
+      </c>
+      <c r="R22" s="18">
+        <v>94.504641532897949</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17">
+        <v>6.8529820442199707</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="18">
+        <v>6.8529820442199707</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17">
+        <v>4.6699457168579102</v>
+      </c>
+      <c r="E24" s="17">
+        <v>5.0735621452331543</v>
+      </c>
+      <c r="F24" s="17">
+        <v>4.5890650749206543</v>
+      </c>
+      <c r="G24" s="17">
+        <v>4.879910945892334</v>
+      </c>
+      <c r="H24" s="17">
+        <v>4.9415140151977539</v>
+      </c>
+      <c r="I24" s="17">
+        <v>4.9939565658569336</v>
+      </c>
+      <c r="J24" s="17">
+        <v>5.0019650459289551</v>
+      </c>
+      <c r="K24" s="17">
+        <v>4.9769253730773926</v>
+      </c>
+      <c r="L24" s="17">
+        <v>5.3125500679016113</v>
+      </c>
+      <c r="M24" s="17">
+        <v>5.5474891662597656</v>
+      </c>
+      <c r="N24" s="17">
+        <v>5.4308328628540039</v>
+      </c>
+      <c r="O24" s="17">
+        <v>5.5942702293395996</v>
+      </c>
+      <c r="P24" s="17">
+        <v>5.8691725730895996</v>
+      </c>
+      <c r="Q24" s="17">
+        <v>6.2677450180053711</v>
+      </c>
+      <c r="R24" s="18">
+        <v>73.148904800415039</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17">
+        <v>4.963742733001709</v>
+      </c>
+      <c r="E25" s="17">
+        <v>5.222867488861084</v>
+      </c>
+      <c r="F25" s="17">
+        <v>5.6187539100646973</v>
+      </c>
+      <c r="G25" s="17">
+        <v>5.1582279205322266</v>
+      </c>
+      <c r="H25" s="17">
+        <v>5.3847732543945313</v>
+      </c>
+      <c r="I25" s="17">
+        <v>5.3887662887573242</v>
+      </c>
+      <c r="J25" s="17">
+        <v>5.6207356452941895</v>
+      </c>
+      <c r="K25" s="17">
+        <v>5.537177562713623</v>
+      </c>
+      <c r="L25" s="17">
+        <v>6.0369768142700195</v>
+      </c>
+      <c r="M25" s="17">
+        <v>5.9955387115478516</v>
+      </c>
+      <c r="N25" s="17">
+        <v>5.8549456596374512</v>
+      </c>
+      <c r="O25" s="17">
+        <v>5.5787429809570313</v>
+      </c>
+      <c r="P25" s="17">
+        <v>5.5135002136230469</v>
+      </c>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="18">
+        <v>71.874749183654785</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="16">
+        <v>7.0796442031860352</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17">
+        <v>7.2666940689086914</v>
+      </c>
+      <c r="F26" s="17">
+        <v>6.8113703727722168</v>
+      </c>
+      <c r="G26" s="17">
+        <v>6.147590160369873</v>
+      </c>
+      <c r="H26" s="17">
+        <v>6.307098388671875</v>
+      </c>
+      <c r="I26" s="17">
+        <v>6.6997895240783691</v>
+      </c>
+      <c r="J26" s="17">
+        <v>6.3963594436645508</v>
+      </c>
+      <c r="K26" s="17">
+        <v>6.4951329231262207</v>
+      </c>
+      <c r="L26" s="17">
+        <v>6.2783780097961426</v>
+      </c>
+      <c r="M26" s="17">
+        <v>6.345491886138916</v>
+      </c>
+      <c r="N26" s="17">
+        <v>6.4739212989807129</v>
+      </c>
+      <c r="O26" s="17">
+        <v>6.2942824363708496</v>
+      </c>
+      <c r="P26" s="17">
+        <v>6.3563933372497559</v>
+      </c>
+      <c r="Q26" s="17">
+        <v>6.5612473487854004</v>
+      </c>
+      <c r="R26" s="18">
+        <v>91.513393402099609</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17">
+        <v>6.462702751159668</v>
+      </c>
+      <c r="E27" s="17">
+        <v>6.8337545394897461</v>
+      </c>
+      <c r="F27" s="17">
+        <v>6.6419568061828613</v>
+      </c>
+      <c r="G27" s="17">
+        <v>6.144676685333252</v>
+      </c>
+      <c r="H27" s="17">
+        <v>6.5314016342163086</v>
+      </c>
+      <c r="I27" s="17">
+        <v>6.5610418319702148</v>
+      </c>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17">
+        <v>6.5332069396972656</v>
+      </c>
+      <c r="L27" s="17">
+        <v>7.0623645782470703</v>
+      </c>
+      <c r="M27" s="17">
+        <v>6.6195249557495117</v>
+      </c>
+      <c r="N27" s="17">
+        <v>6.0334806442260742</v>
+      </c>
+      <c r="O27" s="17">
+        <v>6.3784379959106445</v>
+      </c>
+      <c r="P27" s="17">
+        <v>6.3745641708374023</v>
+      </c>
+      <c r="Q27" s="17">
+        <v>6.3783597946166992</v>
+      </c>
+      <c r="R27" s="18">
+        <v>84.555473327636719</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17">
+        <v>5.083986759185791</v>
+      </c>
+      <c r="E28" s="17">
+        <v>5.2044544219970703</v>
+      </c>
+      <c r="F28" s="17">
+        <v>5.3463068008422852</v>
+      </c>
+      <c r="G28" s="17">
+        <v>5.2184309959411621</v>
+      </c>
+      <c r="H28" s="17">
+        <v>4.6524286270141602</v>
+      </c>
+      <c r="I28" s="17">
+        <v>4.930511474609375</v>
+      </c>
+      <c r="J28" s="17">
+        <v>5.133887767791748</v>
+      </c>
+      <c r="K28" s="17">
+        <v>3.6607272624969482</v>
+      </c>
+      <c r="L28" s="17">
+        <v>4.8284564018249512</v>
+      </c>
+      <c r="M28" s="17">
+        <v>4.8873257637023926</v>
+      </c>
+      <c r="N28" s="17">
+        <v>4.7697396278381348</v>
+      </c>
+      <c r="O28" s="17">
+        <v>4.5136551856994629</v>
+      </c>
+      <c r="P28" s="17">
+        <v>4.8839221000671387</v>
+      </c>
+      <c r="Q28" s="17">
+        <v>5.0348634719848633</v>
+      </c>
+      <c r="R28" s="18">
+        <v>68.148696660995483</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17">
+        <v>5.3321776390075684</v>
+      </c>
+      <c r="E29" s="17">
+        <v>5.7672758102416992</v>
+      </c>
+      <c r="F29" s="17">
+        <v>5.3896245956420898</v>
+      </c>
+      <c r="G29" s="17">
+        <v>5.6476898193359375</v>
+      </c>
+      <c r="H29" s="17">
+        <v>6.1160244941711426</v>
+      </c>
+      <c r="I29" s="17">
+        <v>6.946599006652832</v>
+      </c>
+      <c r="J29" s="17">
+        <v>6.0032868385314941</v>
+      </c>
+      <c r="K29" s="17">
+        <v>5.9588098526000977</v>
+      </c>
+      <c r="L29" s="17">
+        <v>5.8013253211975098</v>
+      </c>
+      <c r="M29" s="17">
+        <v>5.7802114486694336</v>
+      </c>
+      <c r="N29" s="17">
+        <v>5.9705643653869629</v>
+      </c>
+      <c r="O29" s="17">
+        <v>5.8738870620727539</v>
+      </c>
+      <c r="P29" s="17">
+        <v>5.8402314186096191</v>
+      </c>
+      <c r="Q29" s="17">
+        <v>5.9028167724609375</v>
+      </c>
+      <c r="R29" s="18">
+        <v>82.330524444580078</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="16">
+        <v>4.7187337875366211</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17">
+        <v>5.623471736907959</v>
+      </c>
+      <c r="F30" s="17">
+        <v>5.1182317733764648</v>
+      </c>
+      <c r="G30" s="17">
+        <v>5.2128415107727051</v>
+      </c>
+      <c r="H30" s="17">
+        <v>5.4903473854064941</v>
+      </c>
+      <c r="I30" s="17">
+        <v>5.2719440460205078</v>
+      </c>
+      <c r="J30" s="17">
+        <v>5.3090763092041016</v>
+      </c>
+      <c r="K30" s="17">
+        <v>4.8881773948669434</v>
+      </c>
+      <c r="L30" s="17">
+        <v>5.5797944068908691</v>
+      </c>
+      <c r="M30" s="17">
+        <v>5.51446533203125</v>
+      </c>
+      <c r="N30" s="17">
+        <v>5.3262219429016113</v>
+      </c>
+      <c r="O30" s="17">
+        <v>5.607262134552002</v>
+      </c>
+      <c r="P30" s="17">
+        <v>5.1856894493103027</v>
+      </c>
+      <c r="Q30" s="17">
+        <v>4.8720736503601074</v>
+      </c>
+      <c r="R30" s="18">
+        <v>73.718330860137939</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="16">
+        <v>6.9835567474365234</v>
+      </c>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17">
+        <v>6.8019309043884277</v>
+      </c>
+      <c r="F31" s="17">
+        <v>6.9864635467529297</v>
+      </c>
+      <c r="G31" s="17">
+        <v>6.9065470695495605</v>
+      </c>
+      <c r="H31" s="17">
+        <v>7.0293641090393066</v>
+      </c>
+      <c r="I31" s="17">
+        <v>6.8692488670349121</v>
+      </c>
+      <c r="J31" s="17">
+        <v>6.8807840347290039</v>
+      </c>
+      <c r="K31" s="17">
+        <v>6.9180550575256348</v>
+      </c>
+      <c r="L31" s="17">
+        <v>6.7581477165222168</v>
+      </c>
+      <c r="M31" s="17">
+        <v>6.5154452323913574</v>
+      </c>
+      <c r="N31" s="17">
+        <v>6.8242835998535156</v>
+      </c>
+      <c r="O31" s="17">
+        <v>7.1032733917236328</v>
+      </c>
+      <c r="P31" s="17">
+        <v>7.2334451675415039</v>
+      </c>
+      <c r="Q31" s="17">
+        <v>7.1571512222290039</v>
+      </c>
+      <c r="R31" s="18">
+        <v>96.967696666717529</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17">
+        <v>7.1817936897277832</v>
+      </c>
+      <c r="E32" s="17">
+        <v>7.5126876831054688</v>
+      </c>
+      <c r="F32" s="17">
+        <v>7.2803859710693359</v>
+      </c>
+      <c r="G32" s="17">
+        <v>7.1580324172973633</v>
+      </c>
+      <c r="H32" s="17">
+        <v>7.1636161804199219</v>
+      </c>
+      <c r="I32" s="17">
+        <v>7.1151385307312012</v>
+      </c>
+      <c r="J32" s="17">
+        <v>7.0262269973754883</v>
+      </c>
+      <c r="K32" s="17">
+        <v>7.2492852210998535</v>
+      </c>
+      <c r="L32" s="17">
+        <v>7.1511144638061523</v>
+      </c>
+      <c r="M32" s="17">
+        <v>6.8639469146728516</v>
+      </c>
+      <c r="N32" s="17">
+        <v>6.8035998344421387</v>
+      </c>
+      <c r="O32" s="17">
+        <v>6.9917593002319336</v>
+      </c>
+      <c r="P32" s="17">
+        <v>6.8826847076416016</v>
+      </c>
+      <c r="Q32" s="17">
+        <v>6.9437012672424316</v>
+      </c>
+      <c r="R32" s="18">
+        <v>99.323973178863525</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B33" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="20">
+        <v>87.167768478393555</v>
+      </c>
+      <c r="D33" s="21">
+        <v>79.448782444000244</v>
+      </c>
+      <c r="E33" s="21">
+        <v>147.23018264770508</v>
+      </c>
+      <c r="F33" s="21">
+        <v>160.66032838821411</v>
+      </c>
+      <c r="G33" s="21">
+        <v>138.05249881744385</v>
+      </c>
+      <c r="H33" s="21">
+        <v>155.43302774429321</v>
+      </c>
+      <c r="I33" s="21">
+        <v>168.61183071136475</v>
+      </c>
+      <c r="J33" s="21">
+        <v>152.96149826049805</v>
+      </c>
+      <c r="K33" s="21">
+        <v>159.50583100318909</v>
+      </c>
+      <c r="L33" s="21">
+        <v>160.52436351776123</v>
+      </c>
+      <c r="M33" s="21">
+        <v>158.75037622451782</v>
+      </c>
+      <c r="N33" s="21">
+        <v>151.93383073806763</v>
+      </c>
+      <c r="O33" s="21">
+        <v>151.86121129989624</v>
+      </c>
+      <c r="P33" s="21">
+        <v>157.03260350227356</v>
+      </c>
+      <c r="Q33" s="21">
+        <v>153.26932859420776</v>
+      </c>
+      <c r="R33" s="22">
+        <v>2182.4434623718262</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C6:R32">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:Q32">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A066A4D7-296B-4278-A7B3-B8C5BD42EC5E}">
-  <dimension ref="B3:D4"/>
+  <dimension ref="B3:AD29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2007</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2008</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2009</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2010</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
+      <c r="AB7" s="4"/>
+      <c r="AC7" s="4"/>
+      <c r="AD7" s="4"/>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2011</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2012</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="4"/>
+      <c r="AB9" s="4"/>
+      <c r="AC9" s="4"/>
+      <c r="AD9" s="4"/>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2013</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2014</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="4"/>
+      <c r="AD11" s="4"/>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2015</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2016</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="4"/>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4"/>
+      <c r="AD13" s="4"/>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2017</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2018</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
+      <c r="AC15" s="4"/>
+      <c r="AD15" s="4"/>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2019</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="4"/>
+      <c r="AC16" s="4"/>
+      <c r="AD16" s="4"/>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2007</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2008</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2009</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2010</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2011</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2012</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="4"/>
+      <c r="AD22" s="4"/>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2013</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+      <c r="X23" s="4"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="4"/>
+      <c r="AD23" s="4"/>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2014</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="4"/>
+      <c r="AD24" s="4"/>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2015</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="4"/>
+      <c r="AB25" s="4"/>
+      <c r="AC25" s="4"/>
+      <c r="AD25" s="4"/>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2016</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+      <c r="AD26" s="4"/>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2017</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="4">
+        <v>2018</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
+      <c r="AC28" s="4"/>
+      <c r="AD28" s="4"/>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2019</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9DE887-040F-4BFF-8208-44D32E6211A1}">
+  <dimension ref="B3:D6"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,20 +3796,30 @@
         <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>37</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1217,14 +4054,14 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6AEA34B-CA19-4FDB-B38E-0F9FBC5E4E37}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="e1016093-e49d-4fde-a266-0160fb5d213d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
Figured out the bar
</commit_message>
<xml_diff>
--- a/Project Summary.xlsx
+++ b/Project Summary.xlsx
@@ -5,20 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytakeda-my.sharepoint.com/personal/sheri_shojaie_takeda_com/Documents/Documents/__DS Bootcamp/Project/Sheri Sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\com1417\OneDrive - Takeda\Documents\__DS Bootcamp\GitLab\Suicide_squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECFDAA2B-85CC-470C-8E14-910ABCE60162}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="8_{ECFDAA2B-85CC-470C-8E14-910ABCE60162}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4E81A183-2A96-48C0-9EFA-7AB7A9F05363}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{D081F38E-7123-48AD-BD94-A1191E194800}"/>
+    <workbookView xWindow="20040" yWindow="3285" windowWidth="20460" windowHeight="10920" firstSheet="1" activeTab="1" xr2:uid="{D081F38E-7123-48AD-BD94-A1191E194800}"/>
   </bookViews>
   <sheets>
-    <sheet name="Variables" sheetId="1" r:id="rId1"/>
-    <sheet name="Countries" sheetId="2" r:id="rId2"/>
-    <sheet name="Data frame" sheetId="3" r:id="rId3"/>
+    <sheet name="Variables v1" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Task" sheetId="5" r:id="rId2"/>
+    <sheet name="Variables v2" sheetId="4" r:id="rId3"/>
+    <sheet name="Countries" sheetId="2" r:id="rId4"/>
+    <sheet name="Data frame" sheetId="3" r:id="rId5"/>
+    <sheet name="Correlation dataframe" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$B$3:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Variables v1'!$B$3:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Variables v2'!$B$3:$F$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="85">
   <si>
     <t>Independent variable</t>
   </si>
@@ -165,6 +169,133 @@
   </si>
   <si>
     <t>Variable type</t>
+  </si>
+  <si>
+    <t>Variable group</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Happiness index</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Gloom</t>
+  </si>
+  <si>
+    <t>Safety</t>
+  </si>
+  <si>
+    <t>Tourism</t>
+  </si>
+  <si>
+    <t>Data source</t>
+  </si>
+  <si>
+    <t>Vivi</t>
+  </si>
+  <si>
+    <t>Momotaz</t>
+  </si>
+  <si>
+    <t>Almost ready</t>
+  </si>
+  <si>
+    <t>Eben</t>
+  </si>
+  <si>
+    <t>Sheri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task Tracker: </t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To do </t>
+  </si>
+  <si>
+    <t>Data combining</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Clean NaN</t>
+  </si>
+  <si>
+    <t>Sheri + Momo to send data to Vivi for NaN QA</t>
+  </si>
+  <si>
+    <t>Data cleaning: Matrix format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data cleaning: Full dataframe format </t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Question 1: globe</t>
+  </si>
+  <si>
+    <t>Question 2: economic variables (3) x happiness index correlation</t>
+  </si>
+  <si>
+    <t>Question 3: regression for Q2, (if we have time: outliers analysis)</t>
+  </si>
+  <si>
+    <t>Question 4: correlation score for all variables x happiness index</t>
+  </si>
+  <si>
+    <t>Data cleaning: normalize scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data cleaning: NaN </t>
+  </si>
+  <si>
+    <t>Correlation score</t>
+  </si>
+  <si>
+    <t>Question 5a: figure out visualization (multi variable bar chart)</t>
+  </si>
+  <si>
+    <t>Question 5b: load visualization (need data from Q2,3,4)</t>
+  </si>
+  <si>
+    <t>Question 8a: poll: create poll</t>
+  </si>
+  <si>
+    <t>Question 8b: summarize poll results</t>
+  </si>
+  <si>
+    <t>Question 7: globe summary: Showing outlier countries in diff colours
+Dependent on Q2+3</t>
+  </si>
+  <si>
+    <t>Question 7b: conlusion on slide: question 2-5</t>
+  </si>
+  <si>
+    <t>Jkurt + Momo</t>
+  </si>
+  <si>
+    <t>Eben/Sheri</t>
+  </si>
+  <si>
+    <t>OPTIONAL - Question 6a: figure out visualization (violin graph/seaborn library)</t>
+  </si>
+  <si>
+    <t>OPTIONAL - Question 6b: load visualization</t>
   </si>
 </sst>
 </file>
@@ -215,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -225,6 +356,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,407 +674,1336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEA49E3-C43C-47D7-AED7-F4048A0B4EFE}">
-  <dimension ref="B3:G29"/>
+  <dimension ref="B3:H29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="2" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>2019</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>2019</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>2</v>
       </c>
       <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>2</v>
       </c>
       <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>2</v>
       </c>
       <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>2</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>2</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>2018</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:E3" xr:uid="{BCFC110B-267A-44C4-AE1D-9EBD4E8C8E64}"/>
+  <autoFilter ref="B3:F3" xr:uid="{BCFC110B-267A-44C4-AE1D-9EBD4E8C8E64}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D88C2F-CD49-4ACB-B1B1-F9CDCA2543B7}">
+  <dimension ref="B4:F27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="46.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC7E95E-BFCA-4BD0-9E43-BFB2D09E5AAE}">
+  <dimension ref="B3:H28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B3:F3" xr:uid="{BCFC110B-267A-44C4-AE1D-9EBD4E8C8E64}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD03779B-1072-4284-A0C9-AE27034BE457}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -954,7 +2017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A066A4D7-296B-4278-A7B3-B8C5BD42EC5E}">
   <dimension ref="B3:D4"/>
   <sheetViews>
@@ -989,7 +2052,199 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB757E0B-58CD-4CA6-B2F2-0B5402060064}">
+  <dimension ref="B4:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010017584F31B5C7CA498BEC046CF8403204" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ca0af738203bab10c26d8927223bfe4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e1016093-e49d-4fde-a266-0160fb5d213d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7b594759d77e3f213e45e32c2207599" ns3:_="">
     <xsd:import namespace="e1016093-e49d-4fde-a266-0160fb5d213d"/>
@@ -1173,22 +2428,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6AEA34B-CA19-4FDB-B38E-0F9FBC5E4E37}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e1016093-e49d-4fde-a266-0160fb5d213d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA030CA-6F80-4BF5-A231-72E01A2EC08F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA5A59FF-A25B-4B5A-9E2B-D7F1B76B9EC0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1204,28 +2468,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA030CA-6F80-4BF5-A231-72E01A2EC08F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6AEA34B-CA19-4FDB-B38E-0F9FBC5E4E37}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e1016093-e49d-4fde-a266-0160fb5d213d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated Excel tracker and Sheri practice files
</commit_message>
<xml_diff>
--- a/Project Summary.xlsx
+++ b/Project Summary.xlsx
@@ -5,20 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytakeda-my.sharepoint.com/personal/sheri_shojaie_takeda_com/Documents/Documents/__DS Bootcamp/Project/Sheri Sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\com1417\OneDrive - Takeda\Documents\__DS Bootcamp\GitLab\Suicide_squad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECFDAA2B-85CC-470C-8E14-910ABCE60162}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="8_{ECFDAA2B-85CC-470C-8E14-910ABCE60162}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4E81A183-2A96-48C0-9EFA-7AB7A9F05363}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{D081F38E-7123-48AD-BD94-A1191E194800}"/>
+    <workbookView xWindow="20040" yWindow="3285" windowWidth="20460" windowHeight="10920" firstSheet="1" activeTab="1" xr2:uid="{D081F38E-7123-48AD-BD94-A1191E194800}"/>
   </bookViews>
   <sheets>
-    <sheet name="Variables" sheetId="1" r:id="rId1"/>
-    <sheet name="Countries" sheetId="2" r:id="rId2"/>
-    <sheet name="Data frame" sheetId="3" r:id="rId3"/>
+    <sheet name="Variables v1" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Task" sheetId="5" r:id="rId2"/>
+    <sheet name="Variables v2" sheetId="4" r:id="rId3"/>
+    <sheet name="Countries" sheetId="2" r:id="rId4"/>
+    <sheet name="Data frame" sheetId="3" r:id="rId5"/>
+    <sheet name="Correlation dataframe" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$B$3:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Variables v1'!$B$3:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Variables v2'!$B$3:$F$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="85">
   <si>
     <t>Independent variable</t>
   </si>
@@ -165,6 +169,133 @@
   </si>
   <si>
     <t>Variable type</t>
+  </si>
+  <si>
+    <t>Variable group</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Happiness index</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Gloom</t>
+  </si>
+  <si>
+    <t>Safety</t>
+  </si>
+  <si>
+    <t>Tourism</t>
+  </si>
+  <si>
+    <t>Data source</t>
+  </si>
+  <si>
+    <t>Vivi</t>
+  </si>
+  <si>
+    <t>Momotaz</t>
+  </si>
+  <si>
+    <t>Almost ready</t>
+  </si>
+  <si>
+    <t>Eben</t>
+  </si>
+  <si>
+    <t>Sheri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task Tracker: </t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To do </t>
+  </si>
+  <si>
+    <t>Data combining</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Clean NaN</t>
+  </si>
+  <si>
+    <t>Sheri + Momo to send data to Vivi for NaN QA</t>
+  </si>
+  <si>
+    <t>Data cleaning: Matrix format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data cleaning: Full dataframe format </t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Question 1: globe</t>
+  </si>
+  <si>
+    <t>Question 2: economic variables (3) x happiness index correlation</t>
+  </si>
+  <si>
+    <t>Question 3: regression for Q2, (if we have time: outliers analysis)</t>
+  </si>
+  <si>
+    <t>Question 4: correlation score for all variables x happiness index</t>
+  </si>
+  <si>
+    <t>Data cleaning: normalize scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data cleaning: NaN </t>
+  </si>
+  <si>
+    <t>Correlation score</t>
+  </si>
+  <si>
+    <t>Question 5a: figure out visualization (multi variable bar chart)</t>
+  </si>
+  <si>
+    <t>Question 5b: load visualization (need data from Q2,3,4)</t>
+  </si>
+  <si>
+    <t>Question 8a: poll: create poll</t>
+  </si>
+  <si>
+    <t>Question 8b: summarize poll results</t>
+  </si>
+  <si>
+    <t>Question 7: globe summary: Showing outlier countries in diff colours
+Dependent on Q2+3</t>
+  </si>
+  <si>
+    <t>Question 7b: conlusion on slide: question 2-5</t>
+  </si>
+  <si>
+    <t>Jkurt + Momo</t>
+  </si>
+  <si>
+    <t>Eben/Sheri</t>
+  </si>
+  <si>
+    <t>OPTIONAL - Question 6a: figure out visualization (violin graph/seaborn library)</t>
+  </si>
+  <si>
+    <t>OPTIONAL - Question 6b: load visualization</t>
   </si>
 </sst>
 </file>
@@ -215,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -225,6 +356,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,407 +674,1336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEA49E3-C43C-47D7-AED7-F4048A0B4EFE}">
-  <dimension ref="B3:G29"/>
+  <dimension ref="B3:H29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="2" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>2019</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>2019</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>2</v>
       </c>
       <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>2</v>
       </c>
       <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>2</v>
       </c>
       <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>2</v>
       </c>
       <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>2</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>2</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>2018</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:E3" xr:uid="{BCFC110B-267A-44C4-AE1D-9EBD4E8C8E64}"/>
+  <autoFilter ref="B3:F3" xr:uid="{BCFC110B-267A-44C4-AE1D-9EBD4E8C8E64}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D88C2F-CD49-4ACB-B1B1-F9CDCA2543B7}">
+  <dimension ref="B4:F27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="46.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC7E95E-BFCA-4BD0-9E43-BFB2D09E5AAE}">
+  <dimension ref="B3:H28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B3:F3" xr:uid="{BCFC110B-267A-44C4-AE1D-9EBD4E8C8E64}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD03779B-1072-4284-A0C9-AE27034BE457}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -954,7 +2017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A066A4D7-296B-4278-A7B3-B8C5BD42EC5E}">
   <dimension ref="B3:D4"/>
   <sheetViews>
@@ -989,7 +2052,199 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB757E0B-58CD-4CA6-B2F2-0B5402060064}">
+  <dimension ref="B4:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010017584F31B5C7CA498BEC046CF8403204" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ca0af738203bab10c26d8927223bfe4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e1016093-e49d-4fde-a266-0160fb5d213d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a7b594759d77e3f213e45e32c2207599" ns3:_="">
     <xsd:import namespace="e1016093-e49d-4fde-a266-0160fb5d213d"/>
@@ -1173,22 +2428,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6AEA34B-CA19-4FDB-B38E-0F9FBC5E4E37}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e1016093-e49d-4fde-a266-0160fb5d213d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA030CA-6F80-4BF5-A231-72E01A2EC08F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA5A59FF-A25B-4B5A-9E2B-D7F1B76B9EC0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1204,28 +2468,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA030CA-6F80-4BF5-A231-72E01A2EC08F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6AEA34B-CA19-4FDB-B38E-0F9FBC5E4E37}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e1016093-e49d-4fde-a266-0160fb5d213d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>